<commit_message>
Guess I finished questions 1 and 2...
</commit_message>
<xml_diff>
--- a/CIS 450/Assignment 3/Memory Images.xlsx
+++ b/CIS 450/Assignment 3/Memory Images.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
     <t>envp</t>
   </si>
@@ -107,14 +107,269 @@
   </si>
   <si>
     <t>f2</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>LC0</t>
+  </si>
+  <si>
+    <t>%d\11%d\11%d\11%d\12\0</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>f3(22)</t>
+  </si>
+  <si>
+    <t>f2(2)</t>
+  </si>
+  <si>
+    <t>0000000000</t>
+  </si>
+  <si>
+    <t>f1(11)</t>
+  </si>
+  <si>
+    <t>esp(func)</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>trace_me1's fp</t>
+  </si>
+  <si>
+    <t>esp(trace_me1)</t>
+  </si>
+  <si>
+    <t>trace_me1's
+frame</t>
+  </si>
+  <si>
+    <t>n(7)</t>
+  </si>
+  <si>
+    <t>trace_me2's
+frame</t>
+  </si>
+  <si>
+    <t>esp(trace_me2)</t>
+  </si>
+  <si>
+    <t>ret to trace_me1</t>
+  </si>
+  <si>
+    <t>trace_me2's fp</t>
+  </si>
+  <si>
+    <t>%d\t%d\t%d\t%d\t%d\n</t>
+  </si>
+  <si>
+    <t>SG7350</t>
+  </si>
+  <si>
+    <t>SG7359</t>
+  </si>
+  <si>
+    <t>%d\t%d\t%d\n</t>
+  </si>
+  <si>
+    <t>ret to trace_me2</t>
+  </si>
+  <si>
+    <t>n(6)</t>
+  </si>
+  <si>
+    <t>Program Output: 
+2     2     0</t>
+  </si>
+  <si>
+    <t>ret to func</t>
+  </si>
+  <si>
+    <t>Program Output:
+3 2 3 7</t>
+  </si>
+  <si>
+    <r>
+      <t>2,</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1, 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1, 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4, 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1, 2, 1, 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1, 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2, 4, 2</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -420,11 +675,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -495,10 +785,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -507,15 +815,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -548,6 +847,64 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,7 +1189,7 @@
   <dimension ref="B1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,15 +1205,15 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="1">
         <v>16</v>
       </c>
@@ -868,12 +1225,12 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="29" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="30"/>
       <c r="P3" s="1">
         <v>12</v>
@@ -881,17 +1238,21 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="10"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="29" t="s">
+      <c r="C4" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="35"/>
+      <c r="L4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
       <c r="O4" s="30"/>
       <c r="P4" s="1">
         <v>8</v>
@@ -899,17 +1260,21 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="10"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="29" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="49"/>
+      <c r="G5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
       <c r="O5" s="30"/>
       <c r="P5" s="1">
         <v>4</v>
@@ -917,17 +1282,21 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="10"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="29" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
       <c r="O6" s="30"/>
       <c r="P6" s="1" t="s">
         <v>12</v>
@@ -935,79 +1304,83 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="10"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="29" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="53"/>
+      <c r="G7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
       <c r="O7" s="30"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="29" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="30"/>
       <c r="P8" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K9" s="32"/>
-      <c r="L9" s="29" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="10"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="24"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="31"/>
       <c r="O9" s="30"/>
       <c r="P9" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="B10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
       <c r="O10" s="30"/>
       <c r="P10" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="24">
-        <v>8</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="15"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -1017,17 +1390,13 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="24">
-        <v>5</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="32"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="15"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -1036,22 +1405,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="10"/>
-      <c r="J13" s="27" t="s">
+      <c r="C13" s="31">
+        <v>8</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="29">
+      <c r="K13" s="35"/>
+      <c r="L13" s="28">
         <v>9</v>
       </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
       <c r="O13" s="30"/>
       <c r="P13" s="1">
         <v>8</v>
@@ -1062,18 +1435,22 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="10"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="29" t="s">
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="45">
+        <v>5</v>
+      </c>
+      <c r="F14" s="46"/>
+      <c r="G14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="54"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25" t="s">
+      <c r="M14" s="29"/>
+      <c r="N14" s="29" t="s">
         <v>15</v>
       </c>
       <c r="O14" s="30"/>
@@ -1085,21 +1462,23 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="29" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="54"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
       <c r="O15" s="30"/>
       <c r="P15" s="1" t="s">
         <v>17</v>
@@ -1109,30 +1488,40 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J16" s="28"/>
-      <c r="L16" s="29" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="31">
+        <v>3</v>
+      </c>
+      <c r="F16" s="32"/>
+      <c r="G16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="54"/>
+      <c r="L16" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
       <c r="O16" s="30"/>
       <c r="Q16" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="J17" s="28"/>
-      <c r="L17" s="29" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="10"/>
+      <c r="J17" s="54"/>
+      <c r="L17" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
       <c r="O17" s="30"/>
       <c r="Q17" s="1" t="s">
         <v>22</v>
@@ -1140,12 +1529,12 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="10"/>
-      <c r="J18" s="28"/>
+      <c r="J18" s="54"/>
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -1155,15 +1544,13 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="B19" s="9"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="10"/>
-      <c r="J19" s="28"/>
+      <c r="J19" s="54"/>
       <c r="L19" s="20"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -1173,19 +1560,21 @@
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="10"/>
-      <c r="J20" s="28"/>
-      <c r="L20" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="25"/>
-      <c r="N20" s="24" t="s">
-        <v>25</v>
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="J20" s="54"/>
+      <c r="L20" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="29"/>
+      <c r="N20" s="31" t="s">
+        <v>33</v>
       </c>
       <c r="O20" s="30"/>
       <c r="Q20" s="1">
@@ -1193,114 +1582,271 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="L21" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
+      <c r="J21" s="54"/>
+      <c r="L21" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
       <c r="O21" s="30"/>
       <c r="Q21" s="1">
         <v>-16</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="J22" s="54"/>
       <c r="L22" s="20"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
       <c r="O22" s="22"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L23" s="20"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="22"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="54"/>
+      <c r="K23" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L24" s="20"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="10"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="48"/>
+      <c r="N24" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" s="30"/>
+      <c r="P24" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L25" s="20"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="22"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="10"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="30"/>
+      <c r="P25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L26" s="20"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="22"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="30"/>
+      <c r="Q26" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L27" s="20"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="22"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="30"/>
+      <c r="Q27" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K28" s="40"/>
       <c r="L28" s="20"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
       <c r="O28" s="22"/>
+      <c r="Q28" s="1">
+        <v>-4</v>
+      </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="K29" s="40"/>
       <c r="L29" s="20"/>
       <c r="M29" s="21"/>
       <c r="N29" s="21"/>
       <c r="O29" s="22"/>
+      <c r="Q29" s="1">
+        <v>-8</v>
+      </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L30" s="15"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="16"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30" s="29"/>
+      <c r="N30" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="O30" s="30"/>
+      <c r="Q30" s="1">
+        <v>-12</v>
+      </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L31" s="15"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="16"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>-16</v>
+      </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="K32" s="62"/>
       <c r="L32" s="15"/>
       <c r="M32" s="14"/>
       <c r="N32" s="14"/>
       <c r="O32" s="16"/>
     </row>
-    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
+      <c r="K33" s="62"/>
       <c r="L33" s="15"/>
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K34" s="62"/>
       <c r="L34" s="17"/>
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="19"/>
     </row>
-    <row r="35" spans="12:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="62"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="L17:O17"/>
+  <mergeCells count="43">
+    <mergeCell ref="C29:I33"/>
+    <mergeCell ref="K23:K31"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J13:J20"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="L13:O13"/>
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="L14:M14"/>
@@ -1314,6 +1860,15 @@
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="J13:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1322,19 +1877,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="58" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1352,7 +1911,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1363,20 +1922,20 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -1387,84 +1946,96 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="29" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="30"/>
       <c r="P3" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="10"/>
+      <c r="C4" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="29" t="s">
+      <c r="K4" s="35"/>
+      <c r="L4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
       <c r="O4" s="30"/>
       <c r="P4" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="10"/>
+      <c r="C5" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="29" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
       <c r="O5" s="30"/>
       <c r="P5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="29" t="s">
+      <c r="K6" s="35"/>
+      <c r="L6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
       <c r="O6" s="30"/>
       <c r="P6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9"/>
       <c r="C7" s="2"/>
@@ -1474,17 +2045,24 @@
       <c r="G7" s="10"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="J7" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="28">
+        <v>3</v>
+      </c>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
       <c r="O7" s="30"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" s="1">
+        <v>-4</v>
+      </c>
+      <c r="Q7" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="11" t="s">
         <v>6</v>
@@ -1496,17 +2074,22 @@
       <c r="G8" s="13"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="28">
+        <v>4</v>
+      </c>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="30"/>
       <c r="P8" s="1">
         <v>-8</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1516,17 +2099,20 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="1">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" s="54"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1536,57 +2122,79 @@
       <c r="G10" s="8"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="1">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="31">
+        <v>30</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="54"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="15"/>
+      <c r="L11" s="61" t="s">
+        <v>45</v>
+      </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="1">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="58">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="54"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="1">
-        <v>-24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="28">
+        <v>6</v>
+      </c>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="58">
+        <v>-8</v>
+      </c>
+      <c r="R12" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9"/>
       <c r="C13" s="2"/>
@@ -1595,18 +2203,24 @@
       <c r="F13" s="2"/>
       <c r="G13" s="10"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="1"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="55"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="1">
-        <v>-28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="28">
+        <v>3</v>
+      </c>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="58">
+        <v>-12</v>
+      </c>
+      <c r="R13" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9"/>
       <c r="C14" s="2"/>
@@ -1615,18 +2229,21 @@
       <c r="F14" s="2"/>
       <c r="G14" s="10"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="54"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="1">
-        <v>-32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="1"/>
+      <c r="R14" s="58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -1637,18 +2254,21 @@
       <c r="F15" s="12"/>
       <c r="G15" s="13"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="54"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="1">
-        <v>-36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L15" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="1"/>
+      <c r="R15" s="58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1657,18 +2277,26 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="33" t="s">
+        <v>44</v>
+      </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="1">
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L16" s="28">
+        <v>5</v>
+      </c>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="58">
+        <v>12</v>
+      </c>
+      <c r="R16" s="58">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1677,62 +2305,82 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="1">
-        <v>-44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L17" s="28">
+        <v>1</v>
+      </c>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="58">
+        <v>8</v>
+      </c>
+      <c r="R17" s="58">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="10"/>
+      <c r="C18" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="1">
-        <v>-48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L18" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="10"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="54"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="1">
-        <v>-52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1740,17 +2388,20 @@
       <c r="G20" s="10"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="1">
-        <v>-56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="58">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -1759,30 +2410,210 @@
       <c r="F21" s="12"/>
       <c r="G21" s="13"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="1"/>
+      <c r="I21" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="54"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="1">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="L21" s="28">
+        <v>10</v>
+      </c>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="58">
+        <v>-8</v>
+      </c>
+      <c r="R21" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
+      <c r="L22" s="28">
+        <v>0</v>
+      </c>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="30"/>
+      <c r="Q22" s="58">
+        <v>-12</v>
+      </c>
+      <c r="R22" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I23" s="54"/>
+      <c r="L23" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="30"/>
+      <c r="R23" s="58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I24" s="54"/>
+      <c r="L24" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="30"/>
+      <c r="R24" s="58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I25" s="54"/>
+      <c r="L25" s="28">
+        <v>10</v>
+      </c>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="30"/>
+      <c r="R25" s="58">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I26" s="55"/>
+      <c r="L26" s="28">
+        <v>0</v>
+      </c>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="30"/>
+      <c r="R26" s="58">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L27" s="26"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="27"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L28" s="26"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="27"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="27"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="27"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="27"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="27"/>
+    </row>
+    <row r="33" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="15"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="16"/>
+    </row>
+    <row r="34" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L34" s="17"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="19"/>
+    </row>
+    <row r="35" spans="12:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="36">
+    <mergeCell ref="C29:J32"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="I21:I26"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="J16:J22"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="J7:J13"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="K2:K8"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="L12:O12"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L7:O7"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="L7:O7"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="L4:O4"/>
+    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1794,7 +2625,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,15 +2662,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
       <c r="P2" s="1">
         <v>16</v>
       </c>
@@ -1855,12 +2686,12 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="29" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="30"/>
       <c r="P3" s="1">
         <v>12</v>
@@ -1869,20 +2700,20 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="10"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="29" t="s">
+      <c r="K4" s="40"/>
+      <c r="L4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
       <c r="O4" s="30"/>
       <c r="P4" s="1">
         <v>8</v>
@@ -1899,13 +2730,13 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="39" t="s">
+      <c r="K5" s="40"/>
+      <c r="L5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="41"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
       <c r="P5" s="1">
         <v>4</v>
       </c>
@@ -1921,12 +2752,12 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="29" t="s">
+      <c r="K6" s="40"/>
+      <c r="L6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
       <c r="O6" s="30"/>
       <c r="P6" s="1" t="s">
         <v>4</v>
@@ -1943,7 +2774,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="37"/>
+      <c r="K7" s="40"/>
       <c r="L7" s="15"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1965,10 +2796,10 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
       <c r="O8" s="30"/>
       <c r="P8" s="1">
         <v>-8</v>
@@ -1985,10 +2816,10 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
       <c r="O9" s="30"/>
       <c r="P9" s="1">
         <v>-12</v>
@@ -2017,10 +2848,10 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="10"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>

</xml_diff>